<commit_message>
Added kappa by polarity
</commit_message>
<xml_diff>
--- a/Data/results.xlsx
+++ b/Data/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>experiment</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Negative Average</t>
+  </si>
+  <si>
+    <t>Positive only Kappa</t>
+  </si>
+  <si>
+    <t>Mixed only Kappa</t>
+  </si>
+  <si>
+    <t>Negative only Kappa</t>
   </si>
 </sst>
 </file>
@@ -378,11 +387,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="86113792"/>
-        <c:axId val="85069184"/>
+        <c:axId val="82148864"/>
+        <c:axId val="58238080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86113792"/>
+        <c:axId val="82148864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,7 +419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85069184"/>
+        <c:crossAx val="58238080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -418,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85069184"/>
+        <c:axId val="58238080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,7 +466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86113792"/>
+        <c:crossAx val="82148864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -655,11 +664,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="135515648"/>
-        <c:axId val="132321792"/>
+        <c:axId val="82194944"/>
+        <c:axId val="58239808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135515648"/>
+        <c:axId val="82194944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132321792"/>
+        <c:crossAx val="58239808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -695,7 +704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132321792"/>
+        <c:axId val="58239808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -728,7 +737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135515648"/>
+        <c:crossAx val="82194944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,11 +870,11 @@
         </c:dLbls>
         <c:gapWidth val="56"/>
         <c:overlap val="67"/>
-        <c:axId val="3463680"/>
-        <c:axId val="148825216"/>
+        <c:axId val="82195456"/>
+        <c:axId val="58241536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3463680"/>
+        <c:axId val="82195456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -893,7 +902,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148825216"/>
+        <c:crossAx val="58241536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -901,7 +910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148825216"/>
+        <c:axId val="58241536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3463680"/>
+        <c:crossAx val="82195456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1212,11 +1221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="3414528"/>
-        <c:axId val="141233536"/>
+        <c:axId val="82195968"/>
+        <c:axId val="58243264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3414528"/>
+        <c:axId val="82195968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,7 +1253,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141233536"/>
+        <c:crossAx val="58243264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1252,7 +1261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141233536"/>
+        <c:axId val="58243264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1283,7 +1292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3414528"/>
+        <c:crossAx val="82195968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1406,11 +1415,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="78142976"/>
-        <c:axId val="141258112"/>
+        <c:axId val="82196480"/>
+        <c:axId val="84361792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78142976"/>
+        <c:axId val="82196480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1447,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141258112"/>
+        <c:crossAx val="84361792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1446,7 +1455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141258112"/>
+        <c:axId val="84361792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1478,12 +1487,373 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78142976"/>
+        <c:crossAx val="82196480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Positive only Kappa</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$I$21</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Audio Fragments</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audio Full</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AV Fragments</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AV Full</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Text Fragments</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Text Full</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Video Fragments</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Video Full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.64890539999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17715364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59693589999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43155887999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36078757</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26873225000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6496870000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3558319999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mixed only Kappa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$I$21</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Audio Fragments</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audio Full</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AV Fragments</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AV Full</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Text Fragments</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Text Full</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Video Fragments</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Video Full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.50739780000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20278203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51781328000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.37612E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38218785</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7493750000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11599278</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.381642E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Negative only Kappa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$I$21</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Audio Fragments</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audio Full</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AV Fragments</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AV Full</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Text Fragments</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Text Full</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Video Fragments</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Video Full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.79185470000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42564101999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59446659000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14628956000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37527368999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11280100999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.39551E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.311707E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="57673728"/>
+        <c:axId val="129953152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="57673728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Experiment</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129953152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="129953152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>κ</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4897579143389199E-2"/>
+              <c:y val="0.38293251032063208"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57673728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1591,15 +1961,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1620,16 +1990,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1643,6 +2013,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1938,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="W40" sqref="W40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2295,8 +2695,136 @@
         <v>2.95</v>
       </c>
     </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.64890539999999997</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.17715364</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.59693589999999996</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.43155887999999998</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.36078757</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.26873225000000001</v>
+      </c>
+      <c r="H22" s="1">
+        <v>8.6496870000000003E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>4.3558319999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.50739780000000001</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.20278203</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.51781328000000004</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4.37612E-2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.38218785</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2.7493750000000001E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.11599278</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3.381642E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.79185470000000002</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.42564101999999998</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.59446659000000002</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.14628956000000001</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.37527368999999999</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.11280100999999999</v>
+      </c>
+      <c r="H24" s="1">
+        <v>9.39551E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2.311707E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A20:I20"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B7:B8"/>

</xml_diff>

<commit_message>
Removed video 19 from gold file
</commit_message>
<xml_diff>
--- a/Data/results.xlsx
+++ b/Data/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>experiment</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Sigma+spam</t>
   </si>
   <si>
-    <t>Interfragment sigma</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>Negative only Kappa</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>interfragment</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -191,12 +194,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,28 +275,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.65852290000000002</c:v>
+                  <c:v>0.67083391376900003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32718761000000002</c:v>
+                  <c:v>0.326398831188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59219438999999996</c:v>
+                  <c:v>0.59376694489600002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35777352000000001</c:v>
+                  <c:v>0.35960336724699998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38837062</c:v>
+                  <c:v>0.37904764825999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.31190627999999998</c:v>
+                  <c:v>0.283135776053</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.7876169999999998E-2</c:v>
+                  <c:v>9.7876179207099998E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6822449999999997E-2</c:v>
+                  <c:v>5.6822451061E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,28 +348,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.58180580000000004</c:v>
+                  <c:v>0.58180587270799999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13806713000000001</c:v>
+                  <c:v>0.13806713130500001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47368365000000001</c:v>
+                  <c:v>0.47368365871599999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24906423999999999</c:v>
+                  <c:v>0.24906424513700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19287931999999999</c:v>
+                  <c:v>0.192879320794</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23110001999999999</c:v>
+                  <c:v>0.231100026599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.2764480000000006E-2</c:v>
+                  <c:v>7.2764486484600002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.42413805999999998</c:v>
+                  <c:v>-0.42413806950900002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,11 +384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82148864"/>
-        <c:axId val="58238080"/>
+        <c:axId val="43643904"/>
+        <c:axId val="72827456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82148864"/>
+        <c:axId val="43643904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,7 +416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58238080"/>
+        <c:crossAx val="72827456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -427,7 +424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58238080"/>
+        <c:axId val="72827456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82148864"/>
+        <c:crossAx val="43643904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -555,28 +552,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.34336230000000001</c:v>
+                  <c:v>0.33795669076899998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61234191999999998</c:v>
+                  <c:v>0.60529505110100001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42548754999999999</c:v>
+                  <c:v>0.41802112483699999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58129920000000002</c:v>
+                  <c:v>0.574821937921</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50113399000000003</c:v>
+                  <c:v>0.51215863499799996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56583090000000003</c:v>
+                  <c:v>0.62343298237900002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88603217000000001</c:v>
+                  <c:v>0.886032174788</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80918975999999998</c:v>
+                  <c:v>0.80918976863100001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -628,28 +625,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.43028870000000002</c:v>
+                  <c:v>0.43028876079799999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70151699999999995</c:v>
+                  <c:v>0.70151700927799998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54313308000000005</c:v>
+                  <c:v>0.543133086411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63393200999999999</c:v>
+                  <c:v>0.63393201099300001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62201485000000001</c:v>
+                  <c:v>0.62201485296400005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.65499547000000002</c:v>
+                  <c:v>0.65499547209300002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88479074999999996</c:v>
+                  <c:v>0.88479075265899998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83677014000000005</c:v>
+                  <c:v>0.83677014240900005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -664,11 +661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82194944"/>
-        <c:axId val="58239808"/>
+        <c:axId val="80925184"/>
+        <c:axId val="72829184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82194944"/>
+        <c:axId val="80925184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58239808"/>
+        <c:crossAx val="72829184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -704,7 +701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58239808"/>
+        <c:axId val="72829184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -737,7 +734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82194944"/>
+        <c:crossAx val="80925184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -811,16 +808,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.55240460000000002</c:v>
+                  <c:v>0.62087523181500004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57162278</c:v>
+                  <c:v>0.61201236254900004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56395742999999998</c:v>
+                  <c:v>0.55816294858299997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34367872999999999</c:v>
+                  <c:v>0.343678737121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -870,11 +867,11 @@
         </c:dLbls>
         <c:gapWidth val="56"/>
         <c:overlap val="67"/>
-        <c:axId val="82195456"/>
-        <c:axId val="58241536"/>
+        <c:axId val="80926208"/>
+        <c:axId val="72830912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82195456"/>
+        <c:axId val="80926208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -902,7 +899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58241536"/>
+        <c:crossAx val="72830912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -910,7 +907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58241536"/>
+        <c:axId val="72830912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82195456"/>
+        <c:crossAx val="80926208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1029,28 +1026,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.9000409999999999</c:v>
+                  <c:v>3.9629072681699999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3043650700000002</c:v>
+                  <c:v>4.3043650793700001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8046866399999999</c:v>
+                  <c:v>3.8602617655200002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4338744500000002</c:v>
+                  <c:v>4.4338744588700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4998004200000001</c:v>
+                  <c:v>3.6697750229600001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1458333300000003</c:v>
+                  <c:v>4.4090909090899997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4717013799999998</c:v>
+                  <c:v>3.4647173489299998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5668981400000002</c:v>
+                  <c:v>3.5820707070700002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,25 +1104,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.0798412000000002</c:v>
+                  <c:v>3.0116246498599999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.48819444</c:v>
+                  <c:v>3.4881944444399999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1204761900000002</c:v>
+                  <c:v>3.0592436974799999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4392857100000001</c:v>
+                  <c:v>3.43928571429</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.0061497300000002</c:v>
+                  <c:v>3.0070409982199999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.4249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5352941100000002</c:v>
+                  <c:v>3.5352941176499999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.25</c:v>
@@ -1185,25 +1182,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.6928570999999999</c:v>
+                  <c:v>2.6872023809500001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.3687499999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.69222582</c:v>
+                  <c:v>2.6845403439200002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2922619000000002</c:v>
+                  <c:v>2.2922619047600001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7994107700000002</c:v>
+                  <c:v>2.8041456229000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.4500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0550925900000001</c:v>
+                  <c:v>3.0550925925899999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.95</c:v>
@@ -1221,11 +1218,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82195968"/>
-        <c:axId val="58243264"/>
+        <c:axId val="80926720"/>
+        <c:axId val="72832640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82195968"/>
+        <c:axId val="80926720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58243264"/>
+        <c:crossAx val="72832640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1261,7 +1258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58243264"/>
+        <c:axId val="72832640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1292,7 +1289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82195968"/>
+        <c:crossAx val="80926720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1379,28 +1376,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.4909773999999998</c:v>
+                  <c:v>3.5013605442200002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7250417699999998</c:v>
+                  <c:v>3.7721230158700001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4390309100000001</c:v>
+                  <c:v>3.4470143612999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7736215500000001</c:v>
+                  <c:v>3.7992261904800002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2551264999999998</c:v>
+                  <c:v>3.2591718152400002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6625000000000001</c:v>
+                  <c:v>3.7090909090899999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3867724799999999</c:v>
+                  <c:v>3.38677248677</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3801388800000001</c:v>
+                  <c:v>3.3801388888899999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,11 +1412,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82196480"/>
-        <c:axId val="84361792"/>
+        <c:axId val="80927232"/>
+        <c:axId val="85336064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82196480"/>
+        <c:axId val="80927232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84361792"/>
+        <c:crossAx val="85336064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1455,7 +1452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84361792"/>
+        <c:axId val="85336064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1487,7 +1484,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82196480"/>
+        <c:crossAx val="80927232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1572,28 +1569,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.64890539999999997</c:v>
+                  <c:v>0.64198636242999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17715364</c:v>
+                  <c:v>0.177153645936</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59693589999999996</c:v>
+                  <c:v>0.56393243900199996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43155887999999998</c:v>
+                  <c:v>0.431558884325</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36078757</c:v>
+                  <c:v>0.34044254101900001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26873225000000001</c:v>
+                  <c:v>0.16776929601400001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6496870000000003E-2</c:v>
+                  <c:v>8.7882891108800001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3558319999999998E-2</c:v>
+                  <c:v>4.81697589304E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1650,28 +1647,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.50739780000000001</c:v>
+                  <c:v>0.54257044377899999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20278203</c:v>
+                  <c:v>0.20278203000700001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51781328000000004</c:v>
+                  <c:v>0.54495057676000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.37612E-2</c:v>
+                  <c:v>4.37612059234E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38218785</c:v>
+                  <c:v>0.38925197496699998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7493750000000001E-2</c:v>
+                  <c:v>2.74937514201E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11599278</c:v>
+                  <c:v>0.115992783615</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.381642E-2</c:v>
+                  <c:v>3.3816425120799999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1728,28 +1725,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.79185470000000002</c:v>
+                  <c:v>0.79452899658800002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42564101999999998</c:v>
+                  <c:v>0.42564102564099998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59446659000000002</c:v>
+                  <c:v>0.58185328785599999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14628956000000001</c:v>
+                  <c:v>0.14628956758</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37527368999999999</c:v>
+                  <c:v>0.36516106225599998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11280100999999999</c:v>
+                  <c:v>0.112801013942</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.39551E-2</c:v>
+                  <c:v>9.3955107029899995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.311707E-2</c:v>
+                  <c:v>2.31170768084E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1764,11 +1761,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="57673728"/>
-        <c:axId val="129953152"/>
+        <c:axId val="80927744"/>
+        <c:axId val="85337792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57673728"/>
+        <c:axId val="80927744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1796,7 +1793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129953152"/>
+        <c:crossAx val="85337792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1804,7 +1801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129953152"/>
+        <c:axId val="85337792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57673728"/>
+        <c:crossAx val="80927744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1872,12 +1869,12 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -1903,11 +1900,11 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>552449</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -2340,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,149 +2392,157 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.65852290000000002</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.32718761000000002</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.59219438999999996</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.35777352000000001</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.38837062</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.31190627999999998</v>
-      </c>
-      <c r="H3" s="1">
-        <v>9.7876169999999998E-2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>5.6822449999999997E-2</v>
+      <c r="B3">
+        <v>0.67083391376900003</v>
+      </c>
+      <c r="C3">
+        <v>0.326398831188</v>
+      </c>
+      <c r="D3">
+        <v>0.59376694489600002</v>
+      </c>
+      <c r="E3">
+        <v>0.35960336724699998</v>
+      </c>
+      <c r="F3">
+        <v>0.37904764825999998</v>
+      </c>
+      <c r="G3">
+        <v>0.283135776053</v>
+      </c>
+      <c r="H3">
+        <v>9.7876179207099998E-2</v>
+      </c>
+      <c r="I3">
+        <v>5.6822451061E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.58180580000000004</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.13806713000000001</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.47368365000000001</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.24906423999999999</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.19287931999999999</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.23110001999999999</v>
-      </c>
-      <c r="H4" s="1">
-        <v>7.2764480000000006E-2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-0.42413805999999998</v>
+      <c r="B4">
+        <v>0.58180587270799999</v>
+      </c>
+      <c r="C4">
+        <v>0.13806713130500001</v>
+      </c>
+      <c r="D4">
+        <v>0.47368365871599999</v>
+      </c>
+      <c r="E4">
+        <v>0.24906424513700001</v>
+      </c>
+      <c r="F4">
+        <v>0.192879320794</v>
+      </c>
+      <c r="G4">
+        <v>0.231100026599</v>
+      </c>
+      <c r="H4">
+        <v>7.2764486484600002E-2</v>
+      </c>
+      <c r="I4">
+        <v>-0.42413806950900002</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.34336230000000001</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.61234191999999998</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.42548754999999999</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.58129920000000002</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.50113399000000003</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.56583090000000003</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.88603217000000001</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.80918975999999998</v>
+      <c r="B5">
+        <v>0.33795669076899998</v>
+      </c>
+      <c r="C5">
+        <v>0.60529505110100001</v>
+      </c>
+      <c r="D5">
+        <v>0.41802112483699999</v>
+      </c>
+      <c r="E5">
+        <v>0.574821937921</v>
+      </c>
+      <c r="F5">
+        <v>0.51215863499799996</v>
+      </c>
+      <c r="G5">
+        <v>0.62343298237900002</v>
+      </c>
+      <c r="H5">
+        <v>0.886032174788</v>
+      </c>
+      <c r="I5">
+        <v>0.80918976863100001</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.43028870000000002</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.70151699999999995</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.54313308000000005</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.63393200999999999</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.62201485000000001</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.65499547000000002</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.88479074999999996</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.83677014000000005</v>
+      <c r="B6">
+        <v>0.43028876079799999</v>
+      </c>
+      <c r="C6">
+        <v>0.70151700927799998</v>
+      </c>
+      <c r="D6">
+        <v>0.543133086411</v>
+      </c>
+      <c r="E6">
+        <v>0.63393201099300001</v>
+      </c>
+      <c r="F6">
+        <v>0.62201485296400005</v>
+      </c>
+      <c r="G6">
+        <v>0.65499547209300002</v>
+      </c>
+      <c r="H6">
+        <v>0.88479075265899998</v>
+      </c>
+      <c r="I6">
+        <v>0.83677014240900005</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.55240460000000002</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6">
-        <v>0.57162278</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
-        <v>0.56395742999999998</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6">
-        <v>0.34367872999999999</v>
-      </c>
-      <c r="I7" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>0.62087523181500004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>0.61201236254900004</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>0.55816294858299997</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>0.343678737121</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
@@ -2581,117 +2586,117 @@
     </row>
     <row r="13" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3.4909773999999998</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3.7250417699999998</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3.4390309100000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>3.7736215500000001</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3.2551264999999998</v>
-      </c>
-      <c r="G13" s="1">
-        <v>3.6625000000000001</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.3867724799999999</v>
-      </c>
-      <c r="I13" s="1">
-        <v>3.3801388800000001</v>
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>3.5013605442200002</v>
+      </c>
+      <c r="C13">
+        <v>3.7721230158700001</v>
+      </c>
+      <c r="D13">
+        <v>3.4470143612999999</v>
+      </c>
+      <c r="E13">
+        <v>3.7992261904800002</v>
+      </c>
+      <c r="F13">
+        <v>3.2591718152400002</v>
+      </c>
+      <c r="G13">
+        <v>3.7090909090899999</v>
+      </c>
+      <c r="H13">
+        <v>3.38677248677</v>
+      </c>
+      <c r="I13">
+        <v>3.3801388888899999</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>3.9000409999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4.3043650700000002</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3.8046866399999999</v>
-      </c>
-      <c r="E14" s="1">
-        <v>4.4338744500000002</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3.4998004200000001</v>
-      </c>
-      <c r="G14" s="1">
-        <v>4.1458333300000003</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.4717013799999998</v>
-      </c>
-      <c r="I14" s="1">
-        <v>3.5668981400000002</v>
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>3.9629072681699999</v>
+      </c>
+      <c r="C14">
+        <v>4.3043650793700001</v>
+      </c>
+      <c r="D14">
+        <v>3.8602617655200002</v>
+      </c>
+      <c r="E14">
+        <v>4.4338744588700001</v>
+      </c>
+      <c r="F14">
+        <v>3.6697750229600001</v>
+      </c>
+      <c r="G14">
+        <v>4.4090909090899997</v>
+      </c>
+      <c r="H14">
+        <v>3.4647173489299998</v>
+      </c>
+      <c r="I14">
+        <v>3.5820707070700002</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3.0798412000000002</v>
-      </c>
-      <c r="C15" s="1">
-        <v>3.48819444</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3.1204761900000002</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3.4392857100000001</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3.0061497300000002</v>
-      </c>
-      <c r="G15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>3.0116246498599999</v>
+      </c>
+      <c r="C15">
+        <v>3.4881944444399999</v>
+      </c>
+      <c r="D15">
+        <v>3.0592436974799999</v>
+      </c>
+      <c r="E15">
+        <v>3.43928571429</v>
+      </c>
+      <c r="F15">
+        <v>3.0070409982199999</v>
+      </c>
+      <c r="G15">
         <v>3.4249999999999998</v>
       </c>
-      <c r="H15" s="1">
-        <v>3.5352941100000002</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="H15">
+        <v>3.5352941176499999</v>
+      </c>
+      <c r="I15">
         <v>3.25</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2.6928570999999999</v>
-      </c>
-      <c r="C16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2.6872023809500001</v>
+      </c>
+      <c r="C16">
         <v>2.3687499999999999</v>
       </c>
-      <c r="D16" s="1">
-        <v>2.69222582</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2.2922619000000002</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.7994107700000002</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="D16">
+        <v>2.6845403439200002</v>
+      </c>
+      <c r="E16">
+        <v>2.2922619047600001</v>
+      </c>
+      <c r="F16">
+        <v>2.8041456229000001</v>
+      </c>
+      <c r="G16">
         <v>2.4500000000000002</v>
       </c>
-      <c r="H16" s="1">
-        <v>3.0550925900000001</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="H16">
+        <v>3.0550925925899999</v>
+      </c>
+      <c r="I16">
         <v>2.95</v>
       </c>
     </row>
@@ -2737,104 +2742,96 @@
     </row>
     <row r="22" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.64890539999999997</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.17715364</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.59693589999999996</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.43155887999999998</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.36078757</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0.26873225000000001</v>
-      </c>
-      <c r="H22" s="1">
-        <v>8.6496870000000003E-2</v>
-      </c>
-      <c r="I22" s="1">
-        <v>4.3558319999999998E-2</v>
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>0.64198636242999996</v>
+      </c>
+      <c r="C22">
+        <v>0.177153645936</v>
+      </c>
+      <c r="D22">
+        <v>0.56393243900199996</v>
+      </c>
+      <c r="E22">
+        <v>0.431558884325</v>
+      </c>
+      <c r="F22">
+        <v>0.34044254101900001</v>
+      </c>
+      <c r="G22">
+        <v>0.16776929601400001</v>
+      </c>
+      <c r="H22">
+        <v>8.7882891108800001E-2</v>
+      </c>
+      <c r="I22">
+        <v>4.81697589304E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.50739780000000001</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.20278203</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.51781328000000004</v>
-      </c>
-      <c r="E23" s="1">
-        <v>4.37612E-2</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0.38218785</v>
-      </c>
-      <c r="G23" s="1">
-        <v>2.7493750000000001E-2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.11599278</v>
-      </c>
-      <c r="I23" s="1">
-        <v>3.381642E-2</v>
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>0.54257044377899999</v>
+      </c>
+      <c r="C23">
+        <v>0.20278203000700001</v>
+      </c>
+      <c r="D23">
+        <v>0.54495057676000003</v>
+      </c>
+      <c r="E23">
+        <v>4.37612059234E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.38925197496699998</v>
+      </c>
+      <c r="G23">
+        <v>2.74937514201E-2</v>
+      </c>
+      <c r="H23">
+        <v>0.115992783615</v>
+      </c>
+      <c r="I23">
+        <v>3.3816425120799999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.79185470000000002</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.42564101999999998</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.59446659000000002</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.14628956000000001</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0.37527368999999999</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0.11280100999999999</v>
-      </c>
-      <c r="H24" s="1">
-        <v>9.39551E-2</v>
-      </c>
-      <c r="I24" s="1">
-        <v>2.311707E-2</v>
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>0.79452899658800002</v>
+      </c>
+      <c r="C24">
+        <v>0.42564102564099998</v>
+      </c>
+      <c r="D24">
+        <v>0.58185328785599999</v>
+      </c>
+      <c r="E24">
+        <v>0.14628956758</v>
+      </c>
+      <c r="F24">
+        <v>0.36516106225599998</v>
+      </c>
+      <c r="G24">
+        <v>0.112801013942</v>
+      </c>
+      <c r="H24">
+        <v>9.3955107029899995E-2</v>
+      </c>
+      <c r="I24">
+        <v>2.31170768084E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="3">
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>